<commit_message>
first update of 2nd gen
</commit_message>
<xml_diff>
--- a/data/beginner_materials.xlsx
+++ b/data/beginner_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\UPBEAT_studyguide\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\Learning_assistant_AI_tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C72E0C-6684-4500-BED4-58F4B4DC8D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF79884-E816-492F-AE9A-363B875BBABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="2820" windowWidth="35475" windowHeight="18780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="1575" windowWidth="29085" windowHeight="20025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="beginner_materials" sheetId="1" r:id="rId1"/>
@@ -33,33 +33,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Q11.1. Generative AI skills</t>
-  </si>
-  <si>
-    <t>Q11.2. Market Analysis and Customer Understanding</t>
-  </si>
-  <si>
-    <t>Q11.3. Creating and Testing Business Ideas</t>
-  </si>
-  <si>
-    <t>Q11.4. Making a Business Plan</t>
-  </si>
-  <si>
-    <t>Q11.5. Running a Business</t>
-  </si>
-  <si>
-    <t>Q11.6. Branding and Marketing</t>
-  </si>
-  <si>
-    <t>Q11.7. Sales and Customer Service</t>
-  </si>
-  <si>
-    <t>Q11.8. Future-Thinking</t>
-  </si>
-  <si>
-    <t>Q14. General Computer Skills</t>
-  </si>
-  <si>
     <t>If you're looking to improve your computer skills, Microsoft Learn and Google’s Applied Digital Skills offer free tutorials on a range of software and digital tools.</t>
   </si>
   <si>
@@ -101,6 +74,33 @@
     <t>To be able to make an effective business plan, you’ll need some basic knowledge and training on them.
 Learning Resources: Try HubSpot's free "Business Plan Template" and review tutorials on creating business plans on LinkedIn Learning.
 Practice Tip: Draft a mini-business plan, focusing on basic sections such as vision, goals, target audience, and financial projections. You can use generative AI to assist you.</t>
+  </si>
+  <si>
+    <t>Generative AI skills</t>
+  </si>
+  <si>
+    <t>General computer skills</t>
+  </si>
+  <si>
+    <t>Market Analysis and Customer Understanding</t>
+  </si>
+  <si>
+    <t>Creating and Testing Business Ideas</t>
+  </si>
+  <si>
+    <t>Making a Business Plan</t>
+  </si>
+  <si>
+    <t>Running a Business</t>
+  </si>
+  <si>
+    <t>Branding and Marketing</t>
+  </si>
+  <si>
+    <t>Sales and Customer Service</t>
+  </si>
+  <si>
+    <t>Future-Thinking</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -495,74 +495,74 @@
     </row>
     <row r="2" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>